<commit_message>
renew the project names
</commit_message>
<xml_diff>
--- a/project_list/baseProjectInfo.xlsx
+++ b/project_list/baseProjectInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20640" windowHeight="12780"/>
+    <workbookView windowWidth="20670" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,10 +16,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65">
   <si>
-    <t>subject</t>
-  </si>
-  <si>
-    <t>github path</t>
+    <t>Abbr.</t>
+  </si>
+  <si>
+    <t>Subjects</t>
   </si>
   <si>
     <t>SHA</t>
@@ -34,7 +34,7 @@
     <t>lang</t>
   </si>
   <si>
-    <t>apache.commons-lang.meta</t>
+    <t>Apache Commons Lang</t>
   </si>
   <si>
     <t>29495a6dd4088f6f8766699f180a6f9f72c8d8ca</t>
@@ -61,7 +61,7 @@
     <t>uaa</t>
   </si>
   <si>
-    <t>cloudfoundry.uaa.meta</t>
+    <t>UAA</t>
   </si>
   <si>
     <t>abe8e5c5cd9536744773592c370325531feb7644</t>
@@ -79,7 +79,7 @@
     <t>sqlp</t>
   </si>
   <si>
-    <t>FoundationDB.sql-parser.meta</t>
+    <t>Sql Parser</t>
   </si>
   <si>
     <t>e1ecb403c4fa549ad39d513c06bef1e0eb5e2d16</t>
@@ -100,7 +100,7 @@
     <t>joda</t>
   </si>
   <si>
-    <t>JodaOrg.joda-time.meta</t>
+    <t>Joda-Time</t>
   </si>
   <si>
     <t>639c9657af7ff013e64ccfcce6d17a8817330351</t>
@@ -118,7 +118,7 @@
     <t>msg</t>
   </si>
   <si>
-    <t>msgpack.msgpack-java.meta</t>
+    <t>Message Pack for Java</t>
   </si>
   <si>
     <t>83f125635f27332bedd2dc0e60e9635d6ed33e8d</t>
@@ -145,7 +145,7 @@
     <t>apns</t>
   </si>
   <si>
-    <t>notnoop.java-apns.meta</t>
+    <t>Java APNS</t>
   </si>
   <si>
     <t>bb618b107307790ab8a73b2431aefe8c5f2a26f2</t>
@@ -169,7 +169,7 @@
     <t>lafj</t>
   </si>
   <si>
-    <t>vkostyukov.la4j.meta</t>
+    <t>Linear Algebra for Java</t>
   </si>
   <si>
     <t>7bd1091083e7440831d1eab75be76d1b41acf7a6</t>
@@ -196,7 +196,7 @@
     <t>wire</t>
   </si>
   <si>
-    <t>square.wire.meta</t>
+    <t>Wire Mobile Protocol Buffers</t>
   </si>
   <si>
     <t>3cad6d0c67de904776b098a7166994e93c1b8ac8</t>
@@ -216,10 +216,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -661,11 +661,11 @@
         </a:custGeom>
         <a:gradFill rotWithShape="0">
           <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="BBD5F0"/>
+            </a:gs>
             <a:gs pos="100000">
               <a:srgbClr val="9CBEE0"/>
-            </a:gs>
-            <a:gs pos="0">
-              <a:srgbClr val="BBD5F0"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
@@ -692,7 +692,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>

</xml_diff>